<commit_message>
updating the table templates)
</commit_message>
<xml_diff>
--- a/assets/templates/tables.xlsx
+++ b/assets/templates/tables.xlsx
@@ -8,12 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agarr\code\projects\accretion\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{640E31AC-C682-4DBD-90B1-2311623B1130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789849EA-86CE-4A20-8BD3-C56A803C8C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="19200" windowHeight="9970" xr2:uid="{25900BD7-6DE7-4E07-BEF3-FFE8B0EC02B8}"/>
+    <workbookView xWindow="-165" yWindow="-165" windowWidth="38730" windowHeight="21210" activeTab="1" xr2:uid="{25900BD7-6DE7-4E07-BEF3-FFE8B0EC02B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="congress" sheetId="7" r:id="rId2"/>
+    <sheet name="media" sheetId="6" r:id="rId3"/>
+    <sheet name="Achievement" sheetId="5" r:id="rId4"/>
+    <sheet name="Meeting" sheetId="4" r:id="rId5"/>
+    <sheet name="publication" sheetId="3" r:id="rId6"/>
+    <sheet name="New Account" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="52">
   <si>
     <t>office</t>
   </si>
@@ -49,9 +55,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -98,6 +101,102 @@
   </si>
   <si>
     <t>reps/committee</t>
+  </si>
+  <si>
+    <t>contributors (non emp)</t>
+  </si>
+  <si>
+    <t>emp_id is an array</t>
+  </si>
+  <si>
+    <t>off_id is an array</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>asks for</t>
+  </si>
+  <si>
+    <t>first name</t>
+  </si>
+  <si>
+    <t>last name</t>
+  </si>
+  <si>
+    <t>email address</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>office (drop down)</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>title of the paper</t>
+  </si>
+  <si>
+    <t>where is it being published</t>
+  </si>
+  <si>
+    <t>when</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what other usgs employees contribute </t>
+  </si>
+  <si>
+    <t>what non usgs employees contribute</t>
+  </si>
+  <si>
+    <t>these are two fields: first name and last name</t>
+  </si>
+  <si>
+    <t>what meeting are you attending</t>
+  </si>
+  <si>
+    <t>are you presenting any research (if so what is the title)</t>
+  </si>
+  <si>
+    <t>meeting dates</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>what is the achievement?</t>
+  </si>
+  <si>
+    <t>what was the media outlet</t>
+  </si>
+  <si>
+    <t>what was the topic</t>
+  </si>
+  <si>
+    <t>what reps/committee did you meet?</t>
+  </si>
+  <si>
+    <t>what was the topic discussed?</t>
+  </si>
+  <si>
+    <t>did any other employees join you?</t>
+  </si>
+  <si>
+    <t>mtg_date</t>
+  </si>
+  <si>
+    <t>name/desc</t>
+  </si>
+  <si>
+    <t>when?</t>
+  </si>
+  <si>
+    <t>ALL TABLES HAVE A TIMESTAMP</t>
   </si>
 </sst>
 </file>
@@ -240,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -252,6 +351,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,21 +670,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97DABFB-532D-4709-B6EB-50F7A78CE7D6}">
-  <dimension ref="B3:I17"/>
+  <dimension ref="B3:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -588,14 +693,17 @@
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -609,77 +717,92 @@
         <v>3</v>
       </c>
       <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="K4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="D6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="D6" s="2" t="s">
+      <c r="H7" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="7" t="s">
+      <c r="F8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="D9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="F10" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="D7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="D8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="F9" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B13" s="10" t="s">
         <v>3</v>
       </c>
@@ -690,45 +813,450 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B16" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F18" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E853BAA-8143-4EC9-9A91-1D1326B99D51}">
+  <dimension ref="B2:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B9A40A-F09A-4E63-8FBC-F8ECF2A02910}">
+  <dimension ref="B4:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41A5537-2EAB-4483-9EF1-7F9E868346B4}">
+  <dimension ref="B5:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F0040E-1D4D-4123-B2E7-E524FAD186EC}">
+  <dimension ref="B3:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B40C56-2FEA-464A-9B27-EAE62DB5FD0A}">
+  <dimension ref="C3:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C11" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6EDE74-35C9-4C4F-9128-2B7EC44F8BCF}">
+  <dimension ref="B3:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>7</v>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>